<commit_message>
correct xlsx file, for future changes
</commit_message>
<xml_diff>
--- a/ReportGenerator/ReportGenerator/Templates/template.xlsx
+++ b/ReportGenerator/ReportGenerator/Templates/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\(461)Report Generator\ReportGenerator\ReportGenerator\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4945A7D3-ADF8-4449-9D53-39745A0A1913}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D678362-83B1-4D28-90CC-BF94F4CC8C83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -520,7 +520,7 @@
   <dimension ref="A1:M47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1081,8 +1081,8 @@
     <mergeCell ref="A3:I3"/>
     <mergeCell ref="A5:I5"/>
   </mergeCells>
-  <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.19685039370078741" bottom="0.15748031496062992" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <pageMargins left="0.43307086614173229" right="0.43307086614173229" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="90" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>